<commit_message>
feat: Add & update HIV dashboard & complete packages for v. 2.33, 2.34, 2.35, 2.36
</commit_message>
<xml_diff>
--- a/metadata/HIV/HIV_DASHBOARD_V1_DHIS2.33/reference.xlsx
+++ b/metadata/HIV/HIV_DASHBOARD_V1_DHIS2.33/reference.xlsx
@@ -17,6 +17,7 @@
     <sheet name="maps" sheetId="12" r:id="rId12"/>
     <sheet name="legendSets" sheetId="13" r:id="rId13"/>
     <sheet name="userGroups" sheetId="14" r:id="rId14"/>
+    <sheet name="users" sheetId="15" r:id="rId15"/>
   </sheets>
 </workbook>
 </file>
@@ -426,13 +427,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="46.7109375" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -464,7 +465,7 @@
         <v>Version</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>V1.0</v>
+        <v>1.1.0</v>
       </c>
     </row>
     <row r="5">
@@ -472,23 +473,31 @@
         <v>DHIS2 version</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>DHIS2.33</v>
+        <v>2.33.9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>Created</v>
+        <v>DHIS2 build</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>2020-06-11T12:09</v>
+        <v>58094d2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>Identifier</v>
+        <v>Last updated</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>HIV_DASHBOARD_V1.0_DHIS2.33_2020-06-11T12:09</v>
+        <v>20210624T185752</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="str">
+        <v>Name</v>
+      </c>
+      <c r="B8" s="4" t="str">
+        <v>HIV_DASHBOARD_V1.1.0_2.33.9-en</v>
       </c>
     </row>
   </sheetData>
@@ -497,12 +506,12 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="49.7109375" customWidth="1"/>
+    <col min="1" max="1" width="77.7109375" customWidth="1"/>
     <col min="2" max="2" width="224.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
@@ -524,7 +533,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>HIV - 2nd and 3rd 90s</v>
+        <v>HIV - ART coverage - last month</v>
       </c>
       <c r="B2" s="4" t="str">
         <v xml:space="preserve"> </v>
@@ -533,107 +542,135 @@
         <v>2019-06-28</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>YRItoGE02Gc</v>
+        <v>HIeML0i1tW6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>HIV - ART coverage - last month</v>
+        <v>HIV - Proportion of facilities with stockout days for test kits</v>
       </c>
       <c r="B3" s="5" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C3" s="5" t="str">
+        <v>2021-05-03</v>
+      </c>
+      <c r="D3" s="5" t="str">
+        <v>kPE2t8VoO0D</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="str">
+        <v>HIV - Trend in newly diagnosed and new on ART</v>
+      </c>
+      <c r="B4" s="4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C4" s="4" t="str">
+        <v>2020-05-25</v>
+      </c>
+      <c r="D4" s="4" t="str">
+        <v>MlwuLdHcS0Y</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="str">
+        <v>HIV - Trend in HIV test positivity</v>
+      </c>
+      <c r="B5" s="5" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C5" s="5" t="str">
         <v>2019-06-28</v>
       </c>
-      <c r="D3" s="5" t="str">
-        <v>HIeML0i1tW6</v>
-      </c>
-    </row>
-    <row r="4" xml:space="preserve">
-      <c r="A4" s="4" t="str">
+      <c r="D5" s="5" t="str">
+        <v>neY7yCy63LJ</v>
+      </c>
+    </row>
+    <row r="6" xml:space="preserve">
+      <c r="A6" s="4" t="str">
         <v>HIV - HIV cascade</v>
       </c>
-      <c r="B4" s="4" t="str" xml:space="preserve">
+      <c r="B6" s="4" t="str" xml:space="preserve">
         <v xml:space="preserve">HIV positive tests, PLHIV newly on ART and PLHIV retained on treatment over the past 12 months.
 For monitoring HIV programme effectiveness for test and treat policy and retention on treatment over time.</v>
       </c>
-      <c r="C4" s="4" t="str">
+      <c r="C6" s="4" t="str">
         <v>2019-06-28</v>
       </c>
-      <c r="D4" s="4" t="str">
+      <c r="D6" s="4" t="str">
         <v>sbsctgkgtxi</v>
       </c>
     </row>
-    <row r="5" xml:space="preserve">
-      <c r="A5" s="5" t="str">
+    <row r="7">
+      <c r="A7" s="5" t="str">
+        <v>HIV - Trend in HIV testing</v>
+      </c>
+      <c r="B7" s="5" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C7" s="5" t="str">
+        <v>2019-06-28</v>
+      </c>
+      <c r="D7" s="5" t="str">
+        <v>W5YurJlBYxS</v>
+      </c>
+    </row>
+    <row r="8" xml:space="preserve">
+      <c r="A8" s="4" t="str">
         <v>HIV - HIV cascade by gender - last 12 months</v>
       </c>
-      <c r="B5" s="5" t="str" xml:space="preserve">
+      <c r="B8" s="4" t="str" xml:space="preserve">
         <v xml:space="preserve">HIV positive tests, PLHIV newly on ART and PLHIV retained on treatment over the past 12 months by gender.
 For monitoring HIV programme effectiveness for test and treat policy and retention on treatment over time by gender.</v>
       </c>
-      <c r="C5" s="5" t="str">
-        <v>2019-06-28</v>
-      </c>
-      <c r="D5" s="5" t="str">
-        <v>W9BIjYTO9Py</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="str">
-        <v>HIV - Trend in ART retention and VL suppression</v>
-      </c>
-      <c r="B6" s="4" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C6" s="4" t="str">
-        <v>2020-05-25</v>
-      </c>
-      <c r="D6" s="4" t="str">
-        <v>yZx4xQJ1AIt</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="5" t="str">
-        <v>HIV - Trend in HIV test positivity</v>
-      </c>
-      <c r="B7" s="5" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C7" s="5" t="str">
-        <v>2019-06-28</v>
-      </c>
-      <c r="D7" s="5" t="str">
-        <v>neY7yCy63LJ</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="str">
-        <v>HIV - Trend in HIV testing</v>
-      </c>
-      <c r="B8" s="4" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
       <c r="C8" s="4" t="str">
         <v>2019-06-28</v>
       </c>
       <c r="D8" s="4" t="str">
-        <v>W5YurJlBYxS</v>
+        <v>W9BIjYTO9Py</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>HIV - Trend in newly diagnosed and new on ART</v>
+        <v>HIV - Proportion of facilities with stockout days for HIV treatment courses</v>
       </c>
       <c r="B9" s="5" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C9" s="5" t="str">
+        <v>2021-05-03</v>
+      </c>
+      <c r="D9" s="5" t="str">
+        <v>WnqPG2dtDco</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="str">
+        <v>HIV - 2nd and 3rd 90s</v>
+      </c>
+      <c r="B10" s="4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C10" s="4" t="str">
+        <v>2019-06-28</v>
+      </c>
+      <c r="D10" s="4" t="str">
+        <v>YRItoGE02Gc</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="5" t="str">
+        <v>HIV - Trend in ART retention and VL suppression</v>
+      </c>
+      <c r="B11" s="5" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C11" s="5" t="str">
         <v>2020-05-25</v>
       </c>
-      <c r="D9" s="5" t="str">
-        <v>MlwuLdHcS0Y</v>
+      <c r="D11" s="5" t="str">
+        <v>yZx4xQJ1AIt</v>
       </c>
     </row>
   </sheetData>
@@ -642,7 +679,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
@@ -669,21 +706,21 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>HIV - ART coverage by sub-orgunits</v>
+        <v>HIV - ART performance by sub-orgunits</v>
       </c>
       <c r="B2" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2019-06-28</v>
+        <v>2021-06-24</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>FXLnt2rX2GF</v>
+        <v>CInLEIQcstz</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>HIV - ART performance by sub-orgunits</v>
+        <v>HIV - ART coverage by sub-orgunits</v>
       </c>
       <c r="B3" s="5" t="str">
         <v xml:space="preserve"> </v>
@@ -692,20 +729,76 @@
         <v>2019-06-28</v>
       </c>
       <c r="D3" s="5" t="str">
-        <v>CInLEIQcstz</v>
+        <v>FXLnt2rX2GF</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>HIV - HIV testing performance by sub-orgunits</v>
+        <v>HIV - Test kits stock discrepancy</v>
       </c>
       <c r="B4" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>2019-06-28</v>
+        <v>2021-05-03</v>
       </c>
       <c r="D4" s="4" t="str">
+        <v>h34LCgE9DJ8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="str">
+        <v>HIV - Test kits stock status</v>
+      </c>
+      <c r="B5" s="5" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C5" s="5" t="str">
+        <v>2021-05-03</v>
+      </c>
+      <c r="D5" s="5" t="str">
+        <v>kEG0QIt1R5Z</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="str">
+        <v>HIV - Treatment courses stock status</v>
+      </c>
+      <c r="B6" s="4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C6" s="4" t="str">
+        <v>2021-05-10</v>
+      </c>
+      <c r="D6" s="4" t="str">
+        <v>THjGXewUjqC</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="str">
+        <v>HIV - Treatment courses stock discrepancy</v>
+      </c>
+      <c r="B7" s="5" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C7" s="5" t="str">
+        <v>2021-05-03</v>
+      </c>
+      <c r="D7" s="5" t="str">
+        <v>YcsLBRqyW04</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="str">
+        <v>HIV - HIV testing performance by sub-orgunits</v>
+      </c>
+      <c r="B8" s="4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C8" s="4" t="str">
+        <v>2021-06-24</v>
+      </c>
+      <c r="D8" s="4" t="str">
         <v>yM52YmNwPdT</v>
       </c>
     </row>
@@ -715,7 +808,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
@@ -742,21 +835,21 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>GEN - Population estimate</v>
+        <v>HIV - Test kits stockout days by facility</v>
       </c>
       <c r="B2" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2019-06-28</v>
+        <v>2021-05-03</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>Vf3ASwHkAmu</v>
+        <v>apIq7CnXNz6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>HIV - ART coverage</v>
+        <v>HIV - Estimated HIV prevalence</v>
       </c>
       <c r="B3" s="5" t="str">
         <v xml:space="preserve"> </v>
@@ -765,63 +858,119 @@
         <v>2019-06-28</v>
       </c>
       <c r="D3" s="5" t="str">
-        <v>VFaZffBlMro</v>
+        <v>eu3QTttWA2p</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>HIV - ART retention rate (12 months)</v>
+        <v>HIV - Treatment courses stock coverage time by facility</v>
       </c>
       <c r="B4" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>2019-06-28</v>
+        <v>2021-05-03</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v>YLGtwHbfxqG</v>
+        <v>hcf8lXRsRJx</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>HIV - ART retention rate (12 months) by user and sub-orgunits</v>
+        <v>HIV - Test Kits stock coverage time by facility</v>
       </c>
       <c r="B5" s="5" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>2019-06-28</v>
+        <v>2021-05-03</v>
       </c>
       <c r="D5" s="5" t="str">
-        <v>MZMtrkoUQzW</v>
+        <v>jm782q9ElUX</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>HIV - Estimated HIV prevalence</v>
+        <v>HIV - Treatment courses stockout days by facility</v>
       </c>
       <c r="B6" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>2019-06-28</v>
+        <v>2021-05-03</v>
       </c>
       <c r="D6" s="4" t="str">
-        <v>eu3QTttWA2p</v>
+        <v>kpAsHOR1fYq</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>HIV - PLHIV estimate</v>
+        <v>HIV - ART retention rate (12 months) by user and sub-orgunits</v>
       </c>
       <c r="B7" s="5" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C7" s="5" t="str">
+        <v>2021-06-24</v>
+      </c>
+      <c r="D7" s="5" t="str">
+        <v>MZMtrkoUQzW</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="str">
+        <v>HIV - PLHIV estimate</v>
+      </c>
+      <c r="B8" s="4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C8" s="4" t="str">
         <v>2019-06-28</v>
       </c>
-      <c r="D7" s="5" t="str">
+      <c r="D8" s="4" t="str">
         <v>t6lhTAiujEe</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5" t="str">
+        <v>GEN - Population estimate</v>
+      </c>
+      <c r="B9" s="5" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C9" s="5" t="str">
+        <v>2019-06-28</v>
+      </c>
+      <c r="D9" s="5" t="str">
+        <v>Vf3ASwHkAmu</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="str">
+        <v>HIV - ART coverage</v>
+      </c>
+      <c r="B10" s="4" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C10" s="4" t="str">
+        <v>2019-06-28</v>
+      </c>
+      <c r="D10" s="4" t="str">
+        <v>VFaZffBlMro</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="5" t="str">
+        <v>HIV - ART retention rate (12 months)</v>
+      </c>
+      <c r="B11" s="5" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C11" s="5" t="str">
+        <v>2019-06-28</v>
+      </c>
+      <c r="D11" s="5" t="str">
+        <v>YLGtwHbfxqG</v>
       </c>
     </row>
   </sheetData>
@@ -830,17 +979,17 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" customWidth="1"/>
     <col min="4" max="4" width="7.7109375" customWidth="1"/>
     <col min="5" max="5" width="5.7109375" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -884,7 +1033,7 @@
         <v>150</v>
       </c>
       <c r="F2" s="4" t="str">
-        <v>2018-06-29T13:32:27.082</v>
+        <v>2018-06-29</v>
       </c>
       <c r="G2" s="4" t="str">
         <v>ZrYgX2ojLj5</v>
@@ -907,7 +1056,7 @@
         <v>100</v>
       </c>
       <c r="F3" s="5" t="str">
-        <v>2018-06-29T13:32:27.082</v>
+        <v>2018-06-29</v>
       </c>
       <c r="G3" s="5" t="str">
         <v>iCBaHMc9w9O</v>
@@ -930,7 +1079,7 @@
         <v>90</v>
       </c>
       <c r="F4" s="4" t="str">
-        <v>2018-06-29T13:32:27.082</v>
+        <v>2018-06-29</v>
       </c>
       <c r="G4" s="4" t="str">
         <v>bPM6VHCCvzo</v>
@@ -953,7 +1102,7 @@
         <v>75</v>
       </c>
       <c r="F5" s="5" t="str">
-        <v>2018-06-29T13:32:27.081</v>
+        <v>2018-06-29</v>
       </c>
       <c r="G5" s="5" t="str">
         <v>geCVGvs2JPS</v>
@@ -976,10 +1125,194 @@
         <v>60</v>
       </c>
       <c r="F6" s="4" t="str">
-        <v>2018-06-29T13:32:27.082</v>
+        <v>2018-06-29</v>
       </c>
       <c r="G6" s="4" t="str">
         <v>CXStL4SSJ8G</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="str">
+        <v>Stock coverage time</v>
+      </c>
+      <c r="B7" s="5" t="str">
+        <v>f1hWZIYCTzc</v>
+      </c>
+      <c r="C7" s="5" t="str">
+        <v>Invalid</v>
+      </c>
+      <c r="D7" s="5">
+        <v>12</v>
+      </c>
+      <c r="E7" s="5">
+        <v>200</v>
+      </c>
+      <c r="F7" s="5" t="str">
+        <v>2021-04-30</v>
+      </c>
+      <c r="G7" s="5" t="str">
+        <v>wfbGANgbnMR</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="str">
+        <v>Stock coverage time</v>
+      </c>
+      <c r="B8" s="4" t="str">
+        <v>f1hWZIYCTzc</v>
+      </c>
+      <c r="C8" s="4" t="str">
+        <v>Overstock</v>
+      </c>
+      <c r="D8" s="4">
+        <v>3</v>
+      </c>
+      <c r="E8" s="4">
+        <v>12</v>
+      </c>
+      <c r="F8" s="4" t="str">
+        <v>2021-04-30</v>
+      </c>
+      <c r="G8" s="4" t="str">
+        <v>ee8QJxth4ul</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5" t="str">
+        <v>Stock coverage time</v>
+      </c>
+      <c r="B9" s="5" t="str">
+        <v>f1hWZIYCTzc</v>
+      </c>
+      <c r="C9" s="5" t="str">
+        <v>Adequate stock</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5">
+        <v>3</v>
+      </c>
+      <c r="F9" s="5" t="str">
+        <v>2021-04-30</v>
+      </c>
+      <c r="G9" s="5" t="str">
+        <v>mmvDbIcm41d</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="str">
+        <v>Stock coverage time</v>
+      </c>
+      <c r="B10" s="4" t="str">
+        <v>f1hWZIYCTzc</v>
+      </c>
+      <c r="C10" s="4" t="str">
+        <v>Understock</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.0001</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1</v>
+      </c>
+      <c r="F10" s="4" t="str">
+        <v>2021-04-30</v>
+      </c>
+      <c r="G10" s="4" t="str">
+        <v>wAdm1fy3Fmk</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="5" t="str">
+        <v>Stock coverage time</v>
+      </c>
+      <c r="B11" s="5" t="str">
+        <v>f1hWZIYCTzc</v>
+      </c>
+      <c r="C11" s="5" t="str">
+        <v>Stock out</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0.0001</v>
+      </c>
+      <c r="F11" s="5" t="str">
+        <v>2021-04-30</v>
+      </c>
+      <c r="G11" s="5" t="str">
+        <v>fFBIEwglorN</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="str">
+        <v>Stock discrepancy</v>
+      </c>
+      <c r="B12" s="4" t="str">
+        <v>pxeFezcPnQl</v>
+      </c>
+      <c r="C12" s="4" t="str">
+        <v>Positive</v>
+      </c>
+      <c r="D12" s="4">
+        <v>9</v>
+      </c>
+      <c r="E12" s="4">
+        <v>10000000</v>
+      </c>
+      <c r="F12" s="4" t="str">
+        <v>2021-05-11</v>
+      </c>
+      <c r="G12" s="4" t="str">
+        <v>IdLVcKSBYPP</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="5" t="str">
+        <v>Stock discrepancy</v>
+      </c>
+      <c r="B13" s="5" t="str">
+        <v>pxeFezcPnQl</v>
+      </c>
+      <c r="C13" s="5" t="str">
+        <v>Correct stock</v>
+      </c>
+      <c r="D13" s="5">
+        <v>1</v>
+      </c>
+      <c r="E13" s="5">
+        <v>9</v>
+      </c>
+      <c r="F13" s="5" t="str">
+        <v>2021-05-11</v>
+      </c>
+      <c r="G13" s="5" t="str">
+        <v>bW5lmAtDMhX</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="str">
+        <v>Stock discrepancy</v>
+      </c>
+      <c r="B14" s="4" t="str">
+        <v>pxeFezcPnQl</v>
+      </c>
+      <c r="C14" s="4" t="str">
+        <v>Negative</v>
+      </c>
+      <c r="D14" s="4">
+        <v>-10000000</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1</v>
+      </c>
+      <c r="F14" s="4" t="str">
+        <v>2021-05-11</v>
+      </c>
+      <c r="G14" s="4" t="str">
+        <v>EcNjRnWM0Yw</v>
       </c>
     </row>
   </sheetData>
@@ -988,12 +1321,12 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
@@ -1014,7 +1347,7 @@
         <v>HIV access</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-04-24</v>
+        <v>2021-05-20</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>ISvRhzmu8Ck</v>
@@ -1025,21 +1358,48 @@
         <v>HIV admin</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2020-04-24</v>
+        <v>2021-05-20</v>
       </c>
       <c r="C3" s="5" t="str">
         <v>TAVOXarP781</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="4" t="str">
-        <v>HIV data capture</v>
-      </c>
-      <c r="B4" s="4" t="str">
-        <v>2020-05-16</v>
-      </c>
-      <c r="C4" s="4" t="str">
-        <v>OqrNUeHDEQZ</v>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v>Username</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>Last updated</v>
+      </c>
+      <c r="C1" s="3" t="str">
+        <v>UID</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v>who</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <v>2018-07-13</v>
+      </c>
+      <c r="C2" s="4" t="str">
+        <v>vUeLeQMSwhN</v>
       </c>
     </row>
   </sheetData>
@@ -1085,7 +1445,7 @@
         <v>Sex (with unknown)</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2019-06-29</v>
+        <v>2021-02-08</v>
       </c>
       <c r="C3" s="5" t="str">
         <v>XxEFGdwxOJ0</v>
@@ -1102,8 +1462,8 @@
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="28.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
   </cols>
@@ -1124,86 +1484,86 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>[CONFIG] 0-14 years</v>
+        <v>[CONFIG] Female</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>0-14 years</v>
+        <v>Female</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2019-06-28</v>
+        <v>2021-02-08</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>f5VxIY91Jz3</v>
+        <v>bqoVhX2RfG4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>[CONFIG] 15+ years</v>
+        <v>[CONFIG] Male</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>15+ years</v>
+        <v>Male</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>2019-06-29</v>
+        <v>2021-02-08</v>
       </c>
       <c r="D3" s="5" t="str">
-        <v>SqvDE9fTeGl</v>
+        <v>EVYKU2fIc6G</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>[CONFIG] Female</v>
+        <v>[CONFIG] 0-14 years</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>Female</v>
+        <v>0-14 years</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2019-06-28</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v>bqoVhX2RfG4</v>
+        <v>f5VxIY91Jz3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>[CONFIG] Male</v>
+        <v>[CONFIG] 15+ years</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>Male</v>
+        <v>15+ years</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2019-06-29</v>
       </c>
       <c r="D5" s="5" t="str">
-        <v>EVYKU2fIc6G</v>
+        <v>SqvDE9fTeGl</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>[CONFIG] Other/unknown age</v>
+        <v>[CONFIG] Unknown Sex</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>Other/unknown age</v>
+        <v>Unk Sex</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>2019-06-29</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D6" s="4" t="str">
-        <v>YXE2HxNf3YB</v>
+        <v>SZJNeRyrh22</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>[CONFIG] Other/unknown sex</v>
+        <v>[CONFIG] Unknown age</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>Other/unknown sex</v>
+        <v>Unknown age</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>2019-06-29</v>
+        <v>2021-02-08</v>
       </c>
       <c r="D7" s="5" t="str">
-        <v>SZJNeRyrh22</v>
+        <v>YXE2HxNf3YB</v>
       </c>
     </row>
   </sheetData>
@@ -1218,7 +1578,7 @@
   </sheetViews>
   <cols>
     <col min="1" max="1" width="36.7109375" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1250,7 +1610,7 @@
         <v>Age in years  (0-14, 15+, unknown)</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>[CONFIG] Other/unknown age</v>
+        <v>[CONFIG] Unknown age</v>
       </c>
     </row>
     <row r="5">
@@ -1274,7 +1634,7 @@
         <v>Sex (with unknown)</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>[CONFIG] Other/unknown sex</v>
+        <v>[CONFIG] Unknown Sex</v>
       </c>
     </row>
   </sheetData>
@@ -1283,7 +1643,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
@@ -1310,29 +1670,43 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>HIV</v>
+        <v>HIV stock</v>
       </c>
       <c r="B2" s="4" t="str">
         <v/>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2019-06-28</v>
+        <v>2021-05-03</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>HX1nmjQyvdd</v>
+        <v>FFN3XNUfxUJ</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>Population estimates</v>
+        <v>HIV</v>
       </c>
       <c r="B3" s="5" t="str">
         <v/>
       </c>
       <c r="C3" s="5" t="str">
-        <v>2019-06-29</v>
+        <v>2019-06-28</v>
       </c>
       <c r="D3" s="5" t="str">
+        <v>HX1nmjQyvdd</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="str">
+        <v>Population estimates</v>
+      </c>
+      <c r="B4" s="4" t="str">
+        <v/>
+      </c>
+      <c r="C4" s="4" t="str">
+        <v>2021-02-08</v>
+      </c>
+      <c r="D4" s="4" t="str">
         <v>I13HBLJTJMb</v>
       </c>
     </row>
@@ -1342,18 +1716,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="67.7109375" customWidth="1"/>
-    <col min="3" max="3" width="44.7109375" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
-    <col min="5" max="5" width="84.7109375" customWidth="1"/>
-    <col min="6" max="6" width="40.7109375" customWidth="1"/>
-    <col min="7" max="7" width="44.7109375" customWidth="1"/>
+    <col min="2" max="2" width="80.7109375" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" customWidth="1"/>
+    <col min="5" max="5" width="153.7109375" customWidth="1"/>
+    <col min="6" max="6" width="63.7109375" customWidth="1"/>
+    <col min="7" max="7" width="84.7109375" customWidth="1"/>
     <col min="8" max="8" width="25.7109375" customWidth="1"/>
     <col min="9" max="9" width="14.7109375" customWidth="1"/>
     <col min="10" max="10" width="21.7109375" customWidth="1"/>
@@ -1393,22 +1767,22 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>h7bxqdKWYCa</v>
+        <v>aLH7eJpIxvn</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>[CONFIG] GEN - Population total</v>
+        <v>[CONFIG] HIV - PLHIV currently on ART</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>Population</v>
+        <v xml:space="preserve">Currently on ART </v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>GEN_E_POP_TOT</v>
+        <v>HIV_ONART</v>
       </c>
       <c r="E2" s="4" t="str">
-        <v>Estimated total population</v>
+        <v>Number of PLHIV currently on ART</v>
       </c>
       <c r="F2" s="4" t="str">
-        <v>total population</v>
+        <v>PLHIV currently on ART</v>
       </c>
       <c r="G2" s="4" t="str">
         <v>1</v>
@@ -1417,33 +1791,33 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I2" s="4" t="str">
-        <v>2019-06-29</v>
+        <v>2021-06-24</v>
       </c>
       <c r="J2" s="4" t="str">
-        <v>I13HBLJTJMb</v>
+        <v>HX1nmjQyvdd</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>iKW4AMU5YDp</v>
+        <v>bD67D0kVEJQ</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>[CONFIG] HIV - ART coverage rate (%)</v>
+        <v>[CONFIG] HIV - HIV test positivity rate (%)</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>ART coverage (%)</v>
+        <v>HIV test positivity (%)</v>
       </c>
       <c r="D3" s="5" t="str">
-        <v/>
+        <v>HIV_TEST_POSITIVITY</v>
       </c>
       <c r="E3" s="5" t="str">
-        <v/>
+        <v>Percentage of all HIV tests performed that are HIV positive</v>
       </c>
       <c r="F3" s="5" t="str">
-        <v>PLHIV currently receiving ART</v>
+        <v>HIV tests positive</v>
       </c>
       <c r="G3" s="5" t="str">
-        <v>Estimated number of people living with HIV</v>
+        <v>HIV tests performed</v>
       </c>
       <c r="H3" s="5" t="str">
         <v>Percentage</v>
@@ -1457,57 +1831,57 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>JUvYLsNo43H</v>
+        <v>ce0WwqHhVH1</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>[CONFIG] HIV - ART retention rate after 12 months (%)</v>
+        <v>[CONFIG] HIV - HIV test kits discarded</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>ART 12 month retention rate (%)</v>
+        <v>HIV test kits discarded</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v>HIV_ART_12M_RET</v>
+        <v>HIV_HIVTEST_DISCARDED</v>
       </c>
       <c r="E4" s="4" t="str">
-        <v/>
+        <v>Number of HIV test kits discarded during the reporting period (expired, damaged, etc.)</v>
       </c>
       <c r="F4" s="4" t="str">
-        <v>Retained on ART last 12 months</v>
+        <v>HIV test kits discarded</v>
       </c>
       <c r="G4" s="4" t="str">
-        <v>Started ART 12 months ago</v>
+        <v>1</v>
       </c>
       <c r="H4" s="4" t="str">
-        <v>Percentage</v>
+        <v>Numerator only (number)</v>
       </c>
       <c r="I4" s="4" t="str">
-        <v>2019-06-28</v>
+        <v>2020-12-17</v>
       </c>
       <c r="J4" s="4" t="str">
-        <v>HX1nmjQyvdd</v>
+        <v>FFN3XNUfxUJ</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>RnSeEFXobZg</v>
+        <v>drqhQa67F9m</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>[CONFIG] HIV - Estimated HIV prevalence rate (%)</v>
+        <v>[CONFIG] HIV - Ratio of new on ART to newly diagnosed (%)</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>HIV prevalence (%)</v>
+        <v>New on ART to newly diagnosed (%)</v>
       </c>
       <c r="D5" s="5" t="str">
-        <v/>
+        <v>HIV_TREAT</v>
       </c>
       <c r="E5" s="5" t="str">
-        <v>Estimated HIV prevalence rate in percent.</v>
+        <v>Number of new on ART during the period divided by the number of HIV positive tests</v>
       </c>
       <c r="F5" s="5" t="str">
-        <v>Estimated people living with HIV</v>
+        <v>New on ART</v>
       </c>
       <c r="G5" s="5" t="str">
-        <v>Total population</v>
+        <v>HIV tests positive</v>
       </c>
       <c r="H5" s="5" t="str">
         <v>Percentage</v>
@@ -1521,22 +1895,22 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>WJ7pO9GJMNJ</v>
+        <v>ep0DpxsHC6a</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>[CONFIG] HIV - Estimated people living with HIV</v>
+        <v>[CONFIG] HIV - HIV test kits opening balance</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>PLHIV estimate</v>
+        <v>HIV test kits opening balance</v>
       </c>
       <c r="D6" s="4" t="str">
-        <v/>
+        <v>HIV_HIVTEST_OPENING_BALANCE</v>
       </c>
       <c r="E6" s="4" t="str">
-        <v>Number of cases of HIV expected in a geographical area</v>
+        <v>Number of HIV test kits opening balance</v>
       </c>
       <c r="F6" s="4" t="str">
-        <v>HIV - Estimated people living with HIV</v>
+        <v>HIV - HIV test kits opening balance</v>
       </c>
       <c r="G6" s="4" t="str">
         <v>1</v>
@@ -1545,94 +1919,94 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I6" s="4" t="str">
-        <v>2019-06-28</v>
+        <v>2021-02-18</v>
       </c>
       <c r="J6" s="4" t="str">
-        <v>HX1nmjQyvdd</v>
+        <v>FFN3XNUfxUJ</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>bD67D0kVEJQ</v>
+        <v>FI1sLa1hDb1</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>[CONFIG] HIV - HIV test positivity rate (%)</v>
+        <v>[CONFIG] HIV - HIV treatment courses stock out days</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>HIV test positivity (%)</v>
+        <v>HIV treatment courses stock out days</v>
       </c>
       <c r="D7" s="5" t="str">
-        <v>HIV_TEST_POSITIVITY</v>
+        <v>HIV_HIVTX_STOCKOUT_DAYS</v>
       </c>
       <c r="E7" s="5" t="str">
-        <v>Percentage of all HIV tests performed that are HIV positive</v>
+        <v>Number of days when the facility was stocked out of HIV treatment courses (at any point during the day) during the reporting period.</v>
       </c>
       <c r="F7" s="5" t="str">
-        <v>HIV tests positive</v>
+        <v>HIV treatment courses stock out days</v>
       </c>
       <c r="G7" s="5" t="str">
-        <v>HIV tests performed</v>
+        <v>1</v>
       </c>
       <c r="H7" s="5" t="str">
-        <v>Percentage</v>
+        <v>Numerator only (number)</v>
       </c>
       <c r="I7" s="5" t="str">
-        <v>2019-06-28</v>
+        <v>2020-12-17</v>
       </c>
       <c r="J7" s="5" t="str">
-        <v>HX1nmjQyvdd</v>
+        <v>FFN3XNUfxUJ</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>JSUnuftClqK</v>
+        <v>g1wc1mO043P</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>[CONFIG] HIV - HIV tests performed</v>
+        <v>[CONFIG] HIV - Health facilities with HIV treatment courses stock-out days (%)</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>HIV tests performed</v>
+        <v>HF with HIV tx courses stockout days (%)</v>
       </c>
       <c r="D8" s="4" t="str">
-        <v>HIV_TESTS</v>
+        <v>HF_WITH_HIV_TX_COURSES_STOCKOUT_DAYS_%</v>
       </c>
       <c r="E8" s="4" t="str">
-        <v/>
+        <v>Proportion of health facilities with HIV tx courses stockout days</v>
       </c>
       <c r="F8" s="4" t="str">
-        <v>HIV tests performed</v>
+        <v>HF with HIV tx courses stockout days reported</v>
       </c>
       <c r="G8" s="4" t="str">
-        <v>1</v>
+        <v>HF reporting stockout days</v>
       </c>
       <c r="H8" s="4" t="str">
-        <v>Numerator only (number)</v>
+        <v>Percentage</v>
       </c>
       <c r="I8" s="4" t="str">
-        <v>2019-06-28</v>
+        <v>2021-06-10</v>
       </c>
       <c r="J8" s="4" t="str">
-        <v>HX1nmjQyvdd</v>
+        <v>FFN3XNUfxUJ</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>LV138qS9eCD</v>
+        <v>h7bxqdKWYCa</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v xml:space="preserve">[CONFIG] HIV - HIV tests positive </v>
+        <v>[CONFIG] GEN - Population total</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v xml:space="preserve">HIV tests positive </v>
+        <v>Population</v>
       </c>
       <c r="D9" s="5" t="str">
-        <v>HIV_TESTS+</v>
+        <v>GEN_E_POP_TOT</v>
       </c>
       <c r="E9" s="5" t="str">
-        <v>HIV tests found to be positive</v>
+        <v>Estimated total population</v>
       </c>
       <c r="F9" s="5" t="str">
-        <v xml:space="preserve">HIV tests positive </v>
+        <v>total population</v>
       </c>
       <c r="G9" s="5" t="str">
         <v>1</v>
@@ -1641,36 +2015,36 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I9" s="5" t="str">
-        <v>2019-06-28</v>
+        <v>2021-02-08</v>
       </c>
       <c r="J9" s="5" t="str">
-        <v>HX1nmjQyvdd</v>
+        <v>I13HBLJTJMb</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>PTA21lKepjs</v>
+        <v>hcgmW20YI1J</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>[CONFIG] HIV - HIV viral load testing coverage annualized (%)</v>
+        <v xml:space="preserve">[CONFIG] HIV - PLHIV retained on ART last 12 months </v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>Viral load testing coverage annualized (%)</v>
+        <v xml:space="preserve">Retained on ART last 12 months </v>
       </c>
       <c r="D10" s="4" t="str">
-        <v/>
+        <v>HIV_ONART_12M</v>
       </c>
       <c r="E10" s="4" t="str">
         <v/>
       </c>
       <c r="F10" s="4" t="str">
-        <v>PLHIV tested for viral load</v>
+        <v>PLHIV retained on ART last 12 months</v>
       </c>
       <c r="G10" s="4" t="str">
-        <v>PLHIV currently on ART</v>
+        <v>1</v>
       </c>
       <c r="H10" s="4" t="str">
-        <v>Percentage</v>
+        <v>Numerator only (number)</v>
       </c>
       <c r="I10" s="4" t="str">
         <v>2019-06-28</v>
@@ -1681,54 +2055,54 @@
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>aLH7eJpIxvn</v>
+        <v>hwXdEmI1096</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>[CONFIG] HIV - PLHIV currently on ART</v>
+        <v>[CONFIG] HIV - Health facilities with HIV test kits stock-out days (%)</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v xml:space="preserve">Currently on ART </v>
+        <v>HF with HIV test kits stockout days (%)</v>
       </c>
       <c r="D11" s="5" t="str">
-        <v>HIV_ONART</v>
+        <v>HF_WITH_HIV_TEST_KITS_STOCKOUT_DAYS_%</v>
       </c>
       <c r="E11" s="5" t="str">
-        <v/>
+        <v>Proportion of health facilities with HIV test kits stockout days</v>
       </c>
       <c r="F11" s="5" t="str">
-        <v>PLHIV currently on ART</v>
+        <v>HF with HIV test kits stockout days reported</v>
       </c>
       <c r="G11" s="5" t="str">
-        <v>1</v>
+        <v>HF reporting stockout days</v>
       </c>
       <c r="H11" s="5" t="str">
-        <v>Numerator only (number)</v>
+        <v>Percentage</v>
       </c>
       <c r="I11" s="5" t="str">
-        <v>2019-06-28</v>
+        <v>2021-06-10</v>
       </c>
       <c r="J11" s="5" t="str">
-        <v>HX1nmjQyvdd</v>
+        <v>FFN3XNUfxUJ</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>tsMR4m66ili</v>
+        <v>i9siWIY4HDJ</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v xml:space="preserve">[CONFIG] HIV - PLHIV new on ART </v>
+        <v>[CONFIG] HIV - HIV test kits received</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v xml:space="preserve">New on ART </v>
+        <v>HIV test kits received</v>
       </c>
       <c r="D12" s="4" t="str">
-        <v>HIV_ONART_NEW</v>
+        <v>HIV_HIVTEST_RECV</v>
       </c>
       <c r="E12" s="4" t="str">
-        <v/>
+        <v>Number of HIV test kits received</v>
       </c>
       <c r="F12" s="4" t="str">
-        <v>PLHIV new on ART</v>
+        <v>HIV - HIV test kits received</v>
       </c>
       <c r="G12" s="4" t="str">
         <v>1</v>
@@ -1737,36 +2111,36 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I12" s="4" t="str">
-        <v>2019-06-28</v>
+        <v>2021-02-18</v>
       </c>
       <c r="J12" s="4" t="str">
-        <v>HX1nmjQyvdd</v>
+        <v>FFN3XNUfxUJ</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="str">
-        <v>hcgmW20YI1J</v>
+        <v>iKW4AMU5YDp</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v xml:space="preserve">[CONFIG] HIV - PLHIV retained on ART last 12 months </v>
+        <v>[CONFIG] HIV - ART coverage rate (%)</v>
       </c>
       <c r="C13" s="5" t="str">
-        <v xml:space="preserve">Retained on ART last 12 months </v>
+        <v>ART coverage (%)</v>
       </c>
       <c r="D13" s="5" t="str">
-        <v>HIV_ONART_12M</v>
+        <v/>
       </c>
       <c r="E13" s="5" t="str">
         <v/>
       </c>
       <c r="F13" s="5" t="str">
-        <v>PLHIV retained on ART last 12 months</v>
+        <v>PLHIV currently receiving ART</v>
       </c>
       <c r="G13" s="5" t="str">
-        <v>1</v>
+        <v>Estimated number of people living with HIV</v>
       </c>
       <c r="H13" s="5" t="str">
-        <v>Numerator only (number)</v>
+        <v>Percentage</v>
       </c>
       <c r="I13" s="5" t="str">
         <v>2019-06-28</v>
@@ -1777,65 +2151,833 @@
     </row>
     <row r="14">
       <c r="A14" s="4" t="str">
-        <v>zqzX3zcosD5</v>
+        <v>ItdyRTyTGja</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>[CONFIG] HIV - PLHIV tested that are virologically suppressed (%)</v>
+        <v>[CONFIG] HIV - HIV treatment courses opening balance</v>
       </c>
       <c r="C14" s="4" t="str">
-        <v>Virologically suppressed (%)</v>
+        <v>HIV treatment courses opening balance</v>
       </c>
       <c r="D14" s="4" t="str">
-        <v>HIV_TEST_VIRSUPP</v>
+        <v>HIV_HIVTX_OPENING_BALANCE</v>
       </c>
       <c r="E14" s="4" t="str">
-        <v/>
+        <v>Number of HIV treatment courses opening balance</v>
       </c>
       <c r="F14" s="4" t="str">
-        <v>PLHIV virologically suppressed</v>
+        <v>HIV - HIV treatment courses opening balance</v>
       </c>
       <c r="G14" s="4" t="str">
-        <v>PLHIV with viral load tests</v>
+        <v>1</v>
       </c>
       <c r="H14" s="4" t="str">
-        <v>Percentage</v>
+        <v>Numerator only (number)</v>
       </c>
       <c r="I14" s="4" t="str">
-        <v>2019-06-28</v>
+        <v>2021-02-18</v>
       </c>
       <c r="J14" s="4" t="str">
-        <v>HX1nmjQyvdd</v>
+        <v>FFN3XNUfxUJ</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="str">
-        <v>drqhQa67F9m</v>
+        <v>jK4SZrz14cI</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>[CONFIG] HIV - Ratio of new on ART to newly diagnosed (%)</v>
+        <v>[CONFIG] HIV - HIV treatment courses wastage rate (%)</v>
       </c>
       <c r="C15" s="5" t="str">
-        <v>New on ART to newly diagnosed (%)</v>
+        <v>HIV treatment courses wastage rate</v>
       </c>
       <c r="D15" s="5" t="str">
-        <v>HIV_TREAT</v>
+        <v>HIV_TREATMENT_COURSES_WASTAGE_RATE</v>
       </c>
       <c r="E15" s="5" t="str">
-        <v>Number of new on ART during the period divided by the number of HIV positive tests</v>
+        <v>Stock wasted=([Closing balance]-[Stock at hand]) + discarded)</v>
       </c>
       <c r="F15" s="5" t="str">
-        <v>New on ART</v>
+        <v>Stock wasted=([Closing balance]-[Stock at hand]) + discarded)</v>
       </c>
       <c r="G15" s="5" t="str">
-        <v>HIV tests positive</v>
+        <v>Stock used=([Closing balance]-[Stock at hand]) + discarded + dispensed to patient)</v>
       </c>
       <c r="H15" s="5" t="str">
         <v>Percentage</v>
       </c>
       <c r="I15" s="5" t="str">
+        <v>2021-03-21</v>
+      </c>
+      <c r="J15" s="5" t="str">
+        <v>FFN3XNUfxUJ</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="str">
+        <v>Jq21bNzQDq6</v>
+      </c>
+      <c r="B16" s="4" t="str">
+        <v>[CONFIG] HIV - HIV treatment courses stock discrepancy (%)</v>
+      </c>
+      <c r="C16" s="4" t="str">
+        <v>HIV treatment courses stock discrepancy (%)</v>
+      </c>
+      <c r="D16" s="4" t="str">
+        <v>HIV_HIVTX_DISCREPANCY</v>
+      </c>
+      <c r="E16" s="4" t="str">
+        <v>Percentage of the item's stock discrepancy [Stock on hand - Closing balance] / Stock on hand</v>
+      </c>
+      <c r="F16" s="4" t="str">
+        <v>HIV treatment courses stock discrepancy</v>
+      </c>
+      <c r="G16" s="4" t="str">
+        <v>stock on hand</v>
+      </c>
+      <c r="H16" s="4" t="str">
+        <v>Percentage</v>
+      </c>
+      <c r="I16" s="4" t="str">
+        <v>2021-05-11</v>
+      </c>
+      <c r="J16" s="4" t="str">
+        <v>FFN3XNUfxUJ</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="5" t="str">
+        <v>JSUnuftClqK</v>
+      </c>
+      <c r="B17" s="5" t="str">
+        <v>[CONFIG] HIV - HIV tests performed</v>
+      </c>
+      <c r="C17" s="5" t="str">
+        <v>HIV tests performed</v>
+      </c>
+      <c r="D17" s="5" t="str">
+        <v>HIV_TESTS</v>
+      </c>
+      <c r="E17" s="5" t="str">
+        <v>Number of HIV tests performed</v>
+      </c>
+      <c r="F17" s="5" t="str">
+        <v>HIV tests performed</v>
+      </c>
+      <c r="G17" s="5" t="str">
+        <v>1</v>
+      </c>
+      <c r="H17" s="5" t="str">
+        <v>Numerator only (number)</v>
+      </c>
+      <c r="I17" s="5" t="str">
+        <v>2021-06-24</v>
+      </c>
+      <c r="J17" s="5" t="str">
+        <v>HX1nmjQyvdd</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="4" t="str">
+        <v>JUvYLsNo43H</v>
+      </c>
+      <c r="B18" s="4" t="str">
+        <v>[CONFIG] HIV - ART retention rate after 12 months (%)</v>
+      </c>
+      <c r="C18" s="4" t="str">
+        <v>ART 12 month retention rate (%)</v>
+      </c>
+      <c r="D18" s="4" t="str">
+        <v>HIV_ART_12M_RET</v>
+      </c>
+      <c r="E18" s="4" t="str">
+        <v>Proportion of clients on ART retained after 12 months</v>
+      </c>
+      <c r="F18" s="4" t="str">
+        <v>Retained on ART last 12 months</v>
+      </c>
+      <c r="G18" s="4" t="str">
+        <v>Started ART 12 months ago</v>
+      </c>
+      <c r="H18" s="4" t="str">
+        <v>Percentage</v>
+      </c>
+      <c r="I18" s="4" t="str">
+        <v>2021-06-24</v>
+      </c>
+      <c r="J18" s="4" t="str">
+        <v>HX1nmjQyvdd</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="5" t="str">
+        <v>k5oM1u4kpCb</v>
+      </c>
+      <c r="B19" s="5" t="str">
+        <v>[CONFIG] HIV - HIV test kits closing balance</v>
+      </c>
+      <c r="C19" s="5" t="str">
+        <v>HIV test kits closing balance</v>
+      </c>
+      <c r="D19" s="5" t="str">
+        <v>HIV_HIVTEST_CLOSING_BAL</v>
+      </c>
+      <c r="E19" s="5" t="str">
+        <v>Number of HIV test kits as closing balance [Opening balance + Received - Issued - Redistributed - Discarded] at the end of the reporting period</v>
+      </c>
+      <c r="F19" s="5" t="str">
+        <v>HIV test kits closing bal</v>
+      </c>
+      <c r="G19" s="5" t="str">
+        <v>1</v>
+      </c>
+      <c r="H19" s="5" t="str">
+        <v>Numerator only (number)</v>
+      </c>
+      <c r="I19" s="5" t="str">
+        <v>2020-12-17</v>
+      </c>
+      <c r="J19" s="5" t="str">
+        <v>FFN3XNUfxUJ</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="4" t="str">
+        <v>Kc0e1G5Y9lR</v>
+      </c>
+      <c r="B20" s="4" t="str">
+        <v>[CONFIG] HIV - HIV treatment courses redistributed</v>
+      </c>
+      <c r="C20" s="4" t="str">
+        <v>HIV treatment courses redistributed</v>
+      </c>
+      <c r="D20" s="4" t="str">
+        <v>HIV_HIVTX_REDISTRIBUTED</v>
+      </c>
+      <c r="E20" s="4" t="str">
+        <v>Number of HIV treatment courses redistributed</v>
+      </c>
+      <c r="F20" s="4" t="str">
+        <v>HIV - HIV treatment courses redistributed</v>
+      </c>
+      <c r="G20" s="4" t="str">
+        <v>1</v>
+      </c>
+      <c r="H20" s="4" t="str">
+        <v>Numerator only (number)</v>
+      </c>
+      <c r="I20" s="4" t="str">
+        <v>2021-02-18</v>
+      </c>
+      <c r="J20" s="4" t="str">
+        <v>FFN3XNUfxUJ</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="5" t="str">
+        <v>LV138qS9eCD</v>
+      </c>
+      <c r="B21" s="5" t="str">
+        <v xml:space="preserve">[CONFIG] HIV - HIV tests positive </v>
+      </c>
+      <c r="C21" s="5" t="str">
+        <v xml:space="preserve">HIV tests positive </v>
+      </c>
+      <c r="D21" s="5" t="str">
+        <v>HIV_TESTS+</v>
+      </c>
+      <c r="E21" s="5" t="str">
+        <v>HIV tests found to be positive</v>
+      </c>
+      <c r="F21" s="5" t="str">
+        <v xml:space="preserve">HIV tests positive </v>
+      </c>
+      <c r="G21" s="5" t="str">
+        <v>1</v>
+      </c>
+      <c r="H21" s="5" t="str">
+        <v>Numerator only (number)</v>
+      </c>
+      <c r="I21" s="5" t="str">
         <v>2019-06-28</v>
       </c>
-      <c r="J15" s="5" t="str">
+      <c r="J21" s="5" t="str">
+        <v>HX1nmjQyvdd</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="4" t="str">
+        <v>MsRhloUb460</v>
+      </c>
+      <c r="B22" s="4" t="str">
+        <v>[CONFIG] HIV - HIV treatment courses discarded</v>
+      </c>
+      <c r="C22" s="4" t="str">
+        <v>HIV treatment courses discarded</v>
+      </c>
+      <c r="D22" s="4" t="str">
+        <v>HIV_HIVTX_DISCARDED</v>
+      </c>
+      <c r="E22" s="4" t="str">
+        <v>Number of HIV treatment courses discarded during the reporting period (expired, damaged, etc.)</v>
+      </c>
+      <c r="F22" s="4" t="str">
+        <v>HIV treatment courses discarded</v>
+      </c>
+      <c r="G22" s="4" t="str">
+        <v>1</v>
+      </c>
+      <c r="H22" s="4" t="str">
+        <v>Numerator only (number)</v>
+      </c>
+      <c r="I22" s="4" t="str">
+        <v>2020-12-17</v>
+      </c>
+      <c r="J22" s="4" t="str">
+        <v>FFN3XNUfxUJ</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="5" t="str">
+        <v>nqFTRkBEaMd</v>
+      </c>
+      <c r="B23" s="5" t="str">
+        <v>[CONFIG] HIV - HIV treatment courses closing balance</v>
+      </c>
+      <c r="C23" s="5" t="str">
+        <v>HIV treatment courses closing balance</v>
+      </c>
+      <c r="D23" s="5" t="str">
+        <v>HIV_HIVTX_CLOSING_BAL</v>
+      </c>
+      <c r="E23" s="5" t="str">
+        <v>Number of HIV treatment courses as closing balance [Opening balance + Received - Issued - Redistributed - Discarded] at the end of the reporting period</v>
+      </c>
+      <c r="F23" s="5" t="str">
+        <v>HIV treatment courses closing bal</v>
+      </c>
+      <c r="G23" s="5" t="str">
+        <v>1</v>
+      </c>
+      <c r="H23" s="5" t="str">
+        <v>Numerator only (number)</v>
+      </c>
+      <c r="I23" s="5" t="str">
+        <v>2020-12-17</v>
+      </c>
+      <c r="J23" s="5" t="str">
+        <v>FFN3XNUfxUJ</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="4" t="str">
+        <v>PTA21lKepjs</v>
+      </c>
+      <c r="B24" s="4" t="str">
+        <v>[CONFIG] HIV - HIV viral load testing coverage annualized (%)</v>
+      </c>
+      <c r="C24" s="4" t="str">
+        <v>Viral load testing coverage annualized (%)</v>
+      </c>
+      <c r="D24" s="4" t="str">
+        <v>VL_TEST_COV</v>
+      </c>
+      <c r="E24" s="4" t="str">
+        <v>Coverage of HIV viral load testing amongst PLHIV on ART</v>
+      </c>
+      <c r="F24" s="4" t="str">
+        <v>PLHIV tested for viral load</v>
+      </c>
+      <c r="G24" s="4" t="str">
+        <v>PLHIV currently on ART</v>
+      </c>
+      <c r="H24" s="4" t="str">
+        <v>Percentage</v>
+      </c>
+      <c r="I24" s="4" t="str">
+        <v>2021-06-24</v>
+      </c>
+      <c r="J24" s="4" t="str">
+        <v>HX1nmjQyvdd</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="5" t="str">
+        <v>Px6mYqEM8Xx</v>
+      </c>
+      <c r="B25" s="5" t="str">
+        <v>[CONFIG] HIV - Treatment courses stock coverage time</v>
+      </c>
+      <c r="C25" s="5" t="str">
+        <v>HIV Treatment courses stock coverage time</v>
+      </c>
+      <c r="D25" s="5" t="str">
+        <v>HIV_TREATMENT_COURSES_COVERAGE_TIME</v>
+      </c>
+      <c r="E25" s="5" t="str">
+        <v/>
+      </c>
+      <c r="F25" s="5" t="str">
+        <v>usable stock</v>
+      </c>
+      <c r="G25" s="5" t="str">
+        <v>consumed stock</v>
+      </c>
+      <c r="H25" s="5" t="str">
+        <v>Rate (factor=1)</v>
+      </c>
+      <c r="I25" s="5" t="str">
+        <v>2021-05-03</v>
+      </c>
+      <c r="J25" s="5" t="str">
+        <v>FFN3XNUfxUJ</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="4" t="str">
+        <v>qjMG2ZeoioT</v>
+      </c>
+      <c r="B26" s="4" t="str">
+        <v>[CONFIG] HIV - HIV test kits wastage rate (%)</v>
+      </c>
+      <c r="C26" s="4" t="str">
+        <v>HIV test kits wastage rate</v>
+      </c>
+      <c r="D26" s="4" t="str">
+        <v>HIV_TEST_KITS_WASTAGE_RATE</v>
+      </c>
+      <c r="E26" s="4" t="str">
+        <v>Stock wasted=([Closing balance]-[Stock at hand]) + discarded)</v>
+      </c>
+      <c r="F26" s="4" t="str">
+        <v>Stock wasted=([Closing balance]-[Stock at hand]) + discarded)</v>
+      </c>
+      <c r="G26" s="4" t="str">
+        <v>Stock used=([Closing balance]-[Stock at hand]) + discarded + dispensed to patient)</v>
+      </c>
+      <c r="H26" s="4" t="str">
+        <v>Percentage</v>
+      </c>
+      <c r="I26" s="4" t="str">
+        <v>2021-03-21</v>
+      </c>
+      <c r="J26" s="4" t="str">
+        <v>FFN3XNUfxUJ</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="5" t="str">
+        <v>RGetwkZsRXo</v>
+      </c>
+      <c r="B27" s="5" t="str">
+        <v>[CONFIG] HIV - HIV test kits stock discrepancy (%)</v>
+      </c>
+      <c r="C27" s="5" t="str">
+        <v>HIV test kits stock discrepancy (%)</v>
+      </c>
+      <c r="D27" s="5" t="str">
+        <v>HIV_HIVTEST_DISCREPANCY</v>
+      </c>
+      <c r="E27" s="5" t="str">
+        <v>Percentage of the item's stock discrepancy [Stock on hand - Closing balance] / Stock on hand</v>
+      </c>
+      <c r="F27" s="5" t="str">
+        <v>HIV test kits stock discrepancy</v>
+      </c>
+      <c r="G27" s="5" t="str">
+        <v>stock on hand</v>
+      </c>
+      <c r="H27" s="5" t="str">
+        <v>Percentage</v>
+      </c>
+      <c r="I27" s="5" t="str">
+        <v>2021-05-11</v>
+      </c>
+      <c r="J27" s="5" t="str">
+        <v>FFN3XNUfxUJ</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="4" t="str">
+        <v>rL3wP3GneUq</v>
+      </c>
+      <c r="B28" s="4" t="str">
+        <v>[CONFIG] HIV - HIV treatment courses received</v>
+      </c>
+      <c r="C28" s="4" t="str">
+        <v>HIV treatment courses received</v>
+      </c>
+      <c r="D28" s="4" t="str">
+        <v>HIV_HIVTX_RECV</v>
+      </c>
+      <c r="E28" s="4" t="str">
+        <v>Number of HIV treatment courses received</v>
+      </c>
+      <c r="F28" s="4" t="str">
+        <v>HIV - HIV treatment courses received</v>
+      </c>
+      <c r="G28" s="4" t="str">
+        <v>1</v>
+      </c>
+      <c r="H28" s="4" t="str">
+        <v>Numerator only (number)</v>
+      </c>
+      <c r="I28" s="4" t="str">
+        <v>2021-02-18</v>
+      </c>
+      <c r="J28" s="4" t="str">
+        <v>FFN3XNUfxUJ</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="5" t="str">
+        <v>RnSeEFXobZg</v>
+      </c>
+      <c r="B29" s="5" t="str">
+        <v>[CONFIG] HIV - Estimated HIV prevalence rate (%)</v>
+      </c>
+      <c r="C29" s="5" t="str">
+        <v>HIV prevalence (%)</v>
+      </c>
+      <c r="D29" s="5" t="str">
+        <v>HIV_PREV</v>
+      </c>
+      <c r="E29" s="5" t="str">
+        <v>Estimated HIV prevalence rate in percent.</v>
+      </c>
+      <c r="F29" s="5" t="str">
+        <v>Estimated people living with HIV</v>
+      </c>
+      <c r="G29" s="5" t="str">
+        <v>Total population</v>
+      </c>
+      <c r="H29" s="5" t="str">
+        <v>Percentage</v>
+      </c>
+      <c r="I29" s="5" t="str">
+        <v>2021-06-24</v>
+      </c>
+      <c r="J29" s="5" t="str">
+        <v>HX1nmjQyvdd</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="4" t="str">
+        <v>rYRnQKTNqpH</v>
+      </c>
+      <c r="B30" s="4" t="str">
+        <v>[CONFIG] HIV - HIV treatment courses issued</v>
+      </c>
+      <c r="C30" s="4" t="str">
+        <v>HIV treatment courses issued</v>
+      </c>
+      <c r="D30" s="4" t="str">
+        <v>HIV_HIVTX_ISSUED</v>
+      </c>
+      <c r="E30" s="4" t="str">
+        <v>Number of HIV treatment courses issued</v>
+      </c>
+      <c r="F30" s="4" t="str">
+        <v>HIV - HIV treatment courses issued</v>
+      </c>
+      <c r="G30" s="4" t="str">
+        <v>1</v>
+      </c>
+      <c r="H30" s="4" t="str">
+        <v>Numerator only (number)</v>
+      </c>
+      <c r="I30" s="4" t="str">
+        <v>2021-06-11</v>
+      </c>
+      <c r="J30" s="4" t="str">
+        <v>FFN3XNUfxUJ</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="5" t="str">
+        <v>shKUUlxHS8s</v>
+      </c>
+      <c r="B31" s="5" t="str">
+        <v>[CONFIG] HIV - Test kits stock coverage time</v>
+      </c>
+      <c r="C31" s="5" t="str">
+        <v>HIV Test kits stock coverage time</v>
+      </c>
+      <c r="D31" s="5" t="str">
+        <v>HIV_TEST_KITS_COVERAGE_TIME</v>
+      </c>
+      <c r="E31" s="5" t="str">
+        <v/>
+      </c>
+      <c r="F31" s="5" t="str">
+        <v>usable stock</v>
+      </c>
+      <c r="G31" s="5" t="str">
+        <v>consumed stock</v>
+      </c>
+      <c r="H31" s="5" t="str">
+        <v>Rate (factor=1)</v>
+      </c>
+      <c r="I31" s="5" t="str">
+        <v>2021-05-03</v>
+      </c>
+      <c r="J31" s="5" t="str">
+        <v>FFN3XNUfxUJ</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="4" t="str">
+        <v>tKkdc27soF0</v>
+      </c>
+      <c r="B32" s="4" t="str">
+        <v>[CONFIG] HIV - HIV test kits redistributed</v>
+      </c>
+      <c r="C32" s="4" t="str">
+        <v>HIV test kits redistributed</v>
+      </c>
+      <c r="D32" s="4" t="str">
+        <v>HIV_HIVTEST_REDISTRIBUTED</v>
+      </c>
+      <c r="E32" s="4" t="str">
+        <v>Number of HIV test kits redistributed</v>
+      </c>
+      <c r="F32" s="4" t="str">
+        <v>HIV - HIV test kits redistributed</v>
+      </c>
+      <c r="G32" s="4" t="str">
+        <v>1</v>
+      </c>
+      <c r="H32" s="4" t="str">
+        <v>Numerator only (number)</v>
+      </c>
+      <c r="I32" s="4" t="str">
+        <v>2021-02-18</v>
+      </c>
+      <c r="J32" s="4" t="str">
+        <v>FFN3XNUfxUJ</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="5" t="str">
+        <v>tsMR4m66ili</v>
+      </c>
+      <c r="B33" s="5" t="str">
+        <v xml:space="preserve">[CONFIG] HIV - PLHIV new on ART </v>
+      </c>
+      <c r="C33" s="5" t="str">
+        <v xml:space="preserve">New on ART </v>
+      </c>
+      <c r="D33" s="5" t="str">
+        <v>HIV_ONART_NEW</v>
+      </c>
+      <c r="E33" s="5" t="str">
+        <v/>
+      </c>
+      <c r="F33" s="5" t="str">
+        <v>PLHIV new on ART</v>
+      </c>
+      <c r="G33" s="5" t="str">
+        <v>1</v>
+      </c>
+      <c r="H33" s="5" t="str">
+        <v>Numerator only (number)</v>
+      </c>
+      <c r="I33" s="5" t="str">
+        <v>2019-06-28</v>
+      </c>
+      <c r="J33" s="5" t="str">
+        <v>HX1nmjQyvdd</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="4" t="str">
+        <v>wh5KJJPZ2w7</v>
+      </c>
+      <c r="B34" s="4" t="str">
+        <v>[CONFIG] HIV - HIV test kits stock out days</v>
+      </c>
+      <c r="C34" s="4" t="str">
+        <v>HIV test kits stock out days</v>
+      </c>
+      <c r="D34" s="4" t="str">
+        <v>HIV_HIVTEST_STOCKOUT_DAYS</v>
+      </c>
+      <c r="E34" s="4" t="str">
+        <v>Number of days when the facility was stocked out of HIV test kits (at any point during the day) during the reporting period.</v>
+      </c>
+      <c r="F34" s="4" t="str">
+        <v>HIV test kits stock out days</v>
+      </c>
+      <c r="G34" s="4" t="str">
+        <v>1</v>
+      </c>
+      <c r="H34" s="4" t="str">
+        <v>Numerator only (number)</v>
+      </c>
+      <c r="I34" s="4" t="str">
+        <v>2020-12-17</v>
+      </c>
+      <c r="J34" s="4" t="str">
+        <v>FFN3XNUfxUJ</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="5" t="str">
+        <v>WJ7pO9GJMNJ</v>
+      </c>
+      <c r="B35" s="5" t="str">
+        <v>[CONFIG] HIV - Estimated people living with HIV</v>
+      </c>
+      <c r="C35" s="5" t="str">
+        <v>PLHIV estimate</v>
+      </c>
+      <c r="D35" s="5" t="str">
+        <v>PLHIV_EST</v>
+      </c>
+      <c r="E35" s="5" t="str">
+        <v>Number of cases of HIV expected in a geographical area</v>
+      </c>
+      <c r="F35" s="5" t="str">
+        <v>HIV - Estimated people living with HIV</v>
+      </c>
+      <c r="G35" s="5" t="str">
+        <v>1</v>
+      </c>
+      <c r="H35" s="5" t="str">
+        <v>Numerator only (number)</v>
+      </c>
+      <c r="I35" s="5" t="str">
+        <v>2021-06-24</v>
+      </c>
+      <c r="J35" s="5" t="str">
+        <v>HX1nmjQyvdd</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="4" t="str">
+        <v>X6HmDjsA4bt</v>
+      </c>
+      <c r="B36" s="4" t="str">
+        <v>[CONFIG] HIV -HIV test kits stock on hand</v>
+      </c>
+      <c r="C36" s="4" t="str">
+        <v>HIV test kits stock on hand</v>
+      </c>
+      <c r="D36" s="4" t="str">
+        <v>HIV_HIVTEST_STOCK_ON_HAND</v>
+      </c>
+      <c r="E36" s="4" t="str">
+        <v>Number of HIV test kits stock on hand</v>
+      </c>
+      <c r="F36" s="4" t="str">
+        <v>HIV test kits stock on hand</v>
+      </c>
+      <c r="G36" s="4" t="str">
+        <v>1</v>
+      </c>
+      <c r="H36" s="4" t="str">
+        <v>Numerator only (number)</v>
+      </c>
+      <c r="I36" s="4" t="str">
+        <v>2021-03-21</v>
+      </c>
+      <c r="J36" s="4" t="str">
+        <v>FFN3XNUfxUJ</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="5" t="str">
+        <v>Z72mN09tVgx</v>
+      </c>
+      <c r="B37" s="5" t="str">
+        <v>[CONFIG] HIV - HIV treatment courses stock on hand</v>
+      </c>
+      <c r="C37" s="5" t="str">
+        <v>HIV treatment courses stock on hand</v>
+      </c>
+      <c r="D37" s="5" t="str">
+        <v>HIV_HIVTX_STOCK_ON_HAND</v>
+      </c>
+      <c r="E37" s="5" t="str">
+        <v>Number of HIV treatment courses stock on hand</v>
+      </c>
+      <c r="F37" s="5" t="str">
+        <v>HIV - HIV treatment courses stock on hand</v>
+      </c>
+      <c r="G37" s="5" t="str">
+        <v>1</v>
+      </c>
+      <c r="H37" s="5" t="str">
+        <v>Numerator only (number)</v>
+      </c>
+      <c r="I37" s="5" t="str">
+        <v>2021-03-21</v>
+      </c>
+      <c r="J37" s="5" t="str">
+        <v>FFN3XNUfxUJ</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="4" t="str">
+        <v>ZgdUdHnAWmM</v>
+      </c>
+      <c r="B38" s="4" t="str">
+        <v>[CONFIG] HIV - HIV test kits issued</v>
+      </c>
+      <c r="C38" s="4" t="str">
+        <v>HIV test kits issued</v>
+      </c>
+      <c r="D38" s="4" t="str">
+        <v>HIV_HIVTEST_ISSUED</v>
+      </c>
+      <c r="E38" s="4" t="str">
+        <v>Number of HIV test kits issued</v>
+      </c>
+      <c r="F38" s="4" t="str">
+        <v>HIV - HIV test kits issued</v>
+      </c>
+      <c r="G38" s="4" t="str">
+        <v>1</v>
+      </c>
+      <c r="H38" s="4" t="str">
+        <v>Numerator only (number)</v>
+      </c>
+      <c r="I38" s="4" t="str">
+        <v>2021-06-11</v>
+      </c>
+      <c r="J38" s="4" t="str">
+        <v>FFN3XNUfxUJ</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="5" t="str">
+        <v>zqzX3zcosD5</v>
+      </c>
+      <c r="B39" s="5" t="str">
+        <v>[CONFIG] HIV - PLHIV tested that are virologically suppressed (%)</v>
+      </c>
+      <c r="C39" s="5" t="str">
+        <v>Virologically suppressed (%)</v>
+      </c>
+      <c r="D39" s="5" t="str">
+        <v>HIV_TEST_VIRSUPP</v>
+      </c>
+      <c r="E39" s="5" t="str">
+        <v>Proportion of PLHIV tested that are virologically suppressed</v>
+      </c>
+      <c r="F39" s="5" t="str">
+        <v>PLHIV virologically suppressed</v>
+      </c>
+      <c r="G39" s="5" t="str">
+        <v>PLHIV with viral load tests</v>
+      </c>
+      <c r="H39" s="5" t="str">
+        <v>Percentage</v>
+      </c>
+      <c r="I39" s="5" t="str">
+        <v>2021-06-24</v>
+      </c>
+      <c r="J39" s="5" t="str">
         <v>HX1nmjQyvdd</v>
       </c>
     </row>
@@ -1845,7 +2987,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
@@ -1872,30 +3014,44 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>Numerator only (number)</v>
+        <v>Percentage</v>
       </c>
       <c r="B2" s="4">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2018-01-16</v>
+        <v>2021-02-08</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>kHy61PbChXr</v>
+        <v>hmSnCXmLYwt</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>Percentage</v>
+        <v>Rate (factor=1)</v>
       </c>
       <c r="B3" s="5">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>2018-01-16</v>
+        <v>2021-02-08</v>
       </c>
       <c r="D3" s="5" t="str">
-        <v>hmSnCXmLYwt</v>
+        <v>k4RGC3sMTzO</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="str">
+        <v>Numerator only (number)</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4" t="str">
+        <v>2021-02-08</v>
+      </c>
+      <c r="D4" s="4" t="str">
+        <v>kHy61PbChXr</v>
       </c>
     </row>
   </sheetData>
@@ -1904,7 +3060,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
@@ -1927,13 +3083,13 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>HIV Burden</v>
+        <v>HIV Stock</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2019-06-28</v>
+        <v>2021-06-22</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>VjFMk8X026U</v>
+        <v>E20N5NUUk18</v>
       </c>
     </row>
     <row r="3">
@@ -1941,7 +3097,7 @@
         <v>HIV District (SNU2)</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2019-06-28</v>
+        <v>2021-06-24</v>
       </c>
       <c r="C3" s="5" t="str">
         <v>fX1kkuqS47y</v>
@@ -1952,7 +3108,7 @@
         <v>HIV Facility</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>2019-06-28</v>
+        <v>2021-06-24</v>
       </c>
       <c r="C4" s="4" t="str">
         <v>mN578Bop2g3</v>
@@ -1967,6 +3123,17 @@
       </c>
       <c r="C5" s="5" t="str">
         <v>q9qKbXTDgEh</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="str">
+        <v>HIV Burden</v>
+      </c>
+      <c r="B6" s="4" t="str">
+        <v>2019-06-28</v>
+      </c>
+      <c r="C6" s="4" t="str">
+        <v>VjFMk8X026U</v>
       </c>
     </row>
   </sheetData>
@@ -1975,14 +3142,14 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="63.7109375" customWidth="1"/>
+    <col min="3" max="3" width="77.7109375" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
@@ -2010,556 +3177,556 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>Vf3ASwHkAmu</v>
+        <v/>
       </c>
       <c r="B2" s="4" t="str">
-        <v>Map</v>
+        <v>TEXT</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>GEN - Population estimate</v>
+        <v/>
       </c>
       <c r="D2" s="4" t="str">
-        <v>bCMiCx5yJDZ</v>
+        <v>tMeDW1Oc2Io</v>
       </c>
       <c r="E2" s="4" t="str">
-        <v>2019-05-10</v>
+        <v>2021-06-22</v>
       </c>
       <c r="F2" s="4" t="str">
-        <v>VjFMk8X026U</v>
+        <v>E20N5NUUk18</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>t6lhTAiujEe</v>
+        <v>kEG0QIt1R5Z</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>Map</v>
+        <v>Pivot table</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>HIV - PLHIV estimate</v>
+        <v>HIV - Test kits stock status</v>
       </c>
       <c r="D3" s="5" t="str">
-        <v>sXRmIoonkxp</v>
+        <v>yu6ipLd2Y9o</v>
       </c>
       <c r="E3" s="5" t="str">
-        <v>2019-05-10</v>
+        <v>2021-06-22</v>
       </c>
       <c r="F3" s="5" t="str">
-        <v>VjFMk8X026U</v>
+        <v>E20N5NUUk18</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>eu3QTttWA2p</v>
+        <v>h34LCgE9DJ8</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>Map</v>
+        <v>Pivot table</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>HIV - Estimated HIV prevalence</v>
+        <v>HIV - Test kits stock discrepancy</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v>dDuqItmcL36</v>
+        <v>zrYQ6L6gkmV</v>
       </c>
       <c r="E4" s="4" t="str">
-        <v>2019-05-10</v>
+        <v>2021-06-22</v>
       </c>
       <c r="F4" s="4" t="str">
-        <v>VjFMk8X026U</v>
+        <v>E20N5NUUk18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>sbsctgkgtxi</v>
+        <v>jm782q9ElUX</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>Chart</v>
+        <v>Map</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>HIV - HIV cascade</v>
+        <v>HIV - Test Kits stock coverage time by facility</v>
       </c>
       <c r="D5" s="5" t="str">
-        <v>nIA5bdm0wPQ</v>
+        <v>RDFniQYKo6m</v>
       </c>
       <c r="E5" s="5" t="str">
-        <v>2018-07-12</v>
+        <v>2021-06-22</v>
       </c>
       <c r="F5" s="5" t="str">
-        <v>fX1kkuqS47y</v>
+        <v>E20N5NUUk18</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>W9BIjYTO9Py</v>
+        <v>apIq7CnXNz6</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>Chart</v>
+        <v>Map</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>HIV - HIV cascade by gender - last 12 months</v>
+        <v>HIV - Test kits stockout days by facility</v>
       </c>
       <c r="D6" s="4" t="str">
-        <v>uh02i8YxoN2</v>
+        <v>LrsvOXgoxsm</v>
       </c>
       <c r="E6" s="4" t="str">
-        <v>2018-07-11</v>
+        <v>2021-06-22</v>
       </c>
       <c r="F6" s="4" t="str">
-        <v>fX1kkuqS47y</v>
+        <v>E20N5NUUk18</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>YRItoGE02Gc</v>
+        <v>kPE2t8VoO0D</v>
       </c>
       <c r="B7" s="5" t="str">
         <v>Chart</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>HIV - 2nd and 3rd 90s</v>
+        <v>HIV - Proportion of facilities with stockout days for test kits</v>
       </c>
       <c r="D7" s="5" t="str">
-        <v>QZfcLzJWauA</v>
+        <v>HBnQiPWXdYE</v>
       </c>
       <c r="E7" s="5" t="str">
-        <v>2018-07-11</v>
+        <v>2021-06-22</v>
       </c>
       <c r="F7" s="5" t="str">
-        <v>fX1kkuqS47y</v>
+        <v>E20N5NUUk18</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>yM52YmNwPdT</v>
+        <v/>
       </c>
       <c r="B8" s="4" t="str">
-        <v>Pivot table</v>
+        <v>TEXT</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>HIV - HIV testing performance by sub-orgunits</v>
+        <v/>
       </c>
       <c r="D8" s="4" t="str">
-        <v>coEhEClMS5b</v>
+        <v>mD9f0EDRxIw</v>
       </c>
       <c r="E8" s="4" t="str">
-        <v>2018-07-11</v>
+        <v>2021-06-22</v>
       </c>
       <c r="F8" s="4" t="str">
-        <v>fX1kkuqS47y</v>
+        <v>E20N5NUUk18</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>CInLEIQcstz</v>
+        <v>THjGXewUjqC</v>
       </c>
       <c r="B9" s="5" t="str">
         <v>Pivot table</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>HIV - ART performance by sub-orgunits</v>
+        <v>HIV - Treatment courses stock status</v>
       </c>
       <c r="D9" s="5" t="str">
-        <v>JURPIzK3GRR</v>
+        <v>SQn6ArLc1KZ</v>
       </c>
       <c r="E9" s="5" t="str">
-        <v>2018-07-12</v>
+        <v>2021-06-22</v>
       </c>
       <c r="F9" s="5" t="str">
-        <v>fX1kkuqS47y</v>
+        <v>E20N5NUUk18</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>MZMtrkoUQzW</v>
+        <v>YcsLBRqyW04</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>Map</v>
+        <v>Pivot table</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>HIV - ART retention rate (12 months) by user and sub-orgunits</v>
+        <v>HIV - Treatment courses stock discrepancy</v>
       </c>
       <c r="D10" s="4" t="str">
-        <v>iXvO7cOqdAx</v>
+        <v>XdO3FhBLv4m</v>
       </c>
       <c r="E10" s="4" t="str">
-        <v>2018-07-11</v>
+        <v>2021-06-22</v>
       </c>
       <c r="F10" s="4" t="str">
-        <v>fX1kkuqS47y</v>
+        <v>E20N5NUUk18</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>MlwuLdHcS0Y</v>
+        <v>hcf8lXRsRJx</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>Chart</v>
+        <v>Map</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>HIV - Trend in newly diagnosed and new on ART</v>
+        <v>HIV - Treatment courses stock coverage time by facility</v>
       </c>
       <c r="D11" s="5" t="str">
-        <v>uGobU3TTDZZ</v>
+        <v>k8Otq2v8IHO</v>
       </c>
       <c r="E11" s="5" t="str">
-        <v>2018-07-11</v>
+        <v>2021-06-22</v>
       </c>
       <c r="F11" s="5" t="str">
-        <v>fX1kkuqS47y</v>
+        <v>E20N5NUUk18</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>yZx4xQJ1AIt</v>
+        <v>kpAsHOR1fYq</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>Chart</v>
+        <v>Map</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>HIV - Trend in ART retention and VL suppression</v>
+        <v>HIV - Treatment courses stockout days by facility</v>
       </c>
       <c r="D12" s="4" t="str">
-        <v>bj0dK3QOLs2</v>
+        <v>FcoIamaY3rY</v>
       </c>
       <c r="E12" s="4" t="str">
-        <v>2018-07-11</v>
+        <v>2021-06-22</v>
       </c>
       <c r="F12" s="4" t="str">
-        <v>fX1kkuqS47y</v>
+        <v>E20N5NUUk18</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="str">
-        <v>sbsctgkgtxi</v>
+        <v>WnqPG2dtDco</v>
       </c>
       <c r="B13" s="5" t="str">
         <v>Chart</v>
       </c>
       <c r="C13" s="5" t="str">
-        <v>HIV - HIV cascade</v>
+        <v>HIV - Proportion of facilities with stockout days for HIV treatment courses</v>
       </c>
       <c r="D13" s="5" t="str">
-        <v>HQMbQQlWA5L</v>
+        <v>bKKo5hFkIz1</v>
       </c>
       <c r="E13" s="5" t="str">
-        <v>2018-07-12</v>
+        <v>2021-06-22</v>
       </c>
       <c r="F13" s="5" t="str">
-        <v>mN578Bop2g3</v>
+        <v>E20N5NUUk18</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="str">
-        <v>W9BIjYTO9Py</v>
+        <v>sbsctgkgtxi</v>
       </c>
       <c r="B14" s="4" t="str">
         <v>Chart</v>
       </c>
       <c r="C14" s="4" t="str">
-        <v>HIV - HIV cascade by gender - last 12 months</v>
+        <v>HIV - HIV cascade</v>
       </c>
       <c r="D14" s="4" t="str">
-        <v>cQPHqT5WT7k</v>
+        <v>nIA5bdm0wPQ</v>
       </c>
       <c r="E14" s="4" t="str">
-        <v>2018-07-11</v>
+        <v>2021-06-24</v>
       </c>
       <c r="F14" s="4" t="str">
-        <v>mN578Bop2g3</v>
+        <v>fX1kkuqS47y</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="str">
-        <v>YRItoGE02Gc</v>
+        <v>W9BIjYTO9Py</v>
       </c>
       <c r="B15" s="5" t="str">
         <v>Chart</v>
       </c>
       <c r="C15" s="5" t="str">
-        <v>HIV - 2nd and 3rd 90s</v>
+        <v>HIV - HIV cascade by gender - last 12 months</v>
       </c>
       <c r="D15" s="5" t="str">
-        <v>Hn8SpMOfbkR</v>
+        <v>uh02i8YxoN2</v>
       </c>
       <c r="E15" s="5" t="str">
-        <v>2018-07-11</v>
+        <v>2021-06-24</v>
       </c>
       <c r="F15" s="5" t="str">
-        <v>mN578Bop2g3</v>
+        <v>fX1kkuqS47y</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="str">
-        <v>W5YurJlBYxS</v>
+        <v>YRItoGE02Gc</v>
       </c>
       <c r="B16" s="4" t="str">
         <v>Chart</v>
       </c>
       <c r="C16" s="4" t="str">
-        <v>HIV - Trend in HIV testing</v>
+        <v>HIV - 2nd and 3rd 90s</v>
       </c>
       <c r="D16" s="4" t="str">
-        <v>R9mBl80z4gR</v>
+        <v>QZfcLzJWauA</v>
       </c>
       <c r="E16" s="4" t="str">
-        <v>2018-07-11</v>
+        <v>2021-06-24</v>
       </c>
       <c r="F16" s="4" t="str">
-        <v>mN578Bop2g3</v>
+        <v>fX1kkuqS47y</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="5" t="str">
-        <v>neY7yCy63LJ</v>
+        <v>yM52YmNwPdT</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>Chart</v>
+        <v>Pivot table</v>
       </c>
       <c r="C17" s="5" t="str">
-        <v>HIV - Trend in HIV test positivity</v>
+        <v>HIV - HIV testing performance by sub-orgunits</v>
       </c>
       <c r="D17" s="5" t="str">
-        <v>DhGugWmf82U</v>
+        <v>coEhEClMS5b</v>
       </c>
       <c r="E17" s="5" t="str">
-        <v>2018-07-11</v>
+        <v>2021-06-24</v>
       </c>
       <c r="F17" s="5" t="str">
-        <v>mN578Bop2g3</v>
+        <v>fX1kkuqS47y</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="str">
-        <v>MlwuLdHcS0Y</v>
+        <v>CInLEIQcstz</v>
       </c>
       <c r="B18" s="4" t="str">
-        <v>Chart</v>
+        <v>Pivot table</v>
       </c>
       <c r="C18" s="4" t="str">
-        <v>HIV - Trend in newly diagnosed and new on ART</v>
+        <v>HIV - ART performance by sub-orgunits</v>
       </c>
       <c r="D18" s="4" t="str">
-        <v>aOd1P9Jy9Bx</v>
+        <v>JURPIzK3GRR</v>
       </c>
       <c r="E18" s="4" t="str">
-        <v>2018-07-11</v>
+        <v>2021-06-24</v>
       </c>
       <c r="F18" s="4" t="str">
-        <v>mN578Bop2g3</v>
+        <v>fX1kkuqS47y</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="str">
-        <v>yZx4xQJ1AIt</v>
+        <v>MZMtrkoUQzW</v>
       </c>
       <c r="B19" s="5" t="str">
-        <v>Chart</v>
+        <v>Map</v>
       </c>
       <c r="C19" s="5" t="str">
-        <v>HIV - Trend in ART retention and VL suppression</v>
+        <v>HIV - ART retention rate (12 months) by user and sub-orgunits</v>
       </c>
       <c r="D19" s="5" t="str">
-        <v>qCqeB2Is75g</v>
+        <v>iXvO7cOqdAx</v>
       </c>
       <c r="E19" s="5" t="str">
-        <v>2018-07-11</v>
+        <v>2021-06-24</v>
       </c>
       <c r="F19" s="5" t="str">
-        <v>mN578Bop2g3</v>
+        <v>fX1kkuqS47y</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="str">
-        <v>sbsctgkgtxi</v>
+        <v>MlwuLdHcS0Y</v>
       </c>
       <c r="B20" s="4" t="str">
         <v>Chart</v>
       </c>
       <c r="C20" s="4" t="str">
-        <v>HIV - HIV cascade</v>
+        <v>HIV - Trend in newly diagnosed and new on ART</v>
       </c>
       <c r="D20" s="4" t="str">
-        <v>jnd7OXSZ3td</v>
+        <v>uGobU3TTDZZ</v>
       </c>
       <c r="E20" s="4" t="str">
-        <v>2019-05-10</v>
+        <v>2021-06-24</v>
       </c>
       <c r="F20" s="4" t="str">
-        <v>q9qKbXTDgEh</v>
+        <v>fX1kkuqS47y</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="5" t="str">
-        <v>W9BIjYTO9Py</v>
+        <v>yZx4xQJ1AIt</v>
       </c>
       <c r="B21" s="5" t="str">
         <v>Chart</v>
       </c>
       <c r="C21" s="5" t="str">
-        <v>HIV - HIV cascade by gender - last 12 months</v>
+        <v>HIV - Trend in ART retention and VL suppression</v>
       </c>
       <c r="D21" s="5" t="str">
-        <v>XnNRP887MgT</v>
+        <v>bj0dK3QOLs2</v>
       </c>
       <c r="E21" s="5" t="str">
-        <v>2019-05-10</v>
+        <v>2021-06-24</v>
       </c>
       <c r="F21" s="5" t="str">
-        <v>q9qKbXTDgEh</v>
+        <v>fX1kkuqS47y</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="str">
-        <v>YRItoGE02Gc</v>
+        <v>sbsctgkgtxi</v>
       </c>
       <c r="B22" s="4" t="str">
         <v>Chart</v>
       </c>
       <c r="C22" s="4" t="str">
-        <v>HIV - 2nd and 3rd 90s</v>
+        <v>HIV - HIV cascade</v>
       </c>
       <c r="D22" s="4" t="str">
-        <v>Yybjz35BBy4</v>
+        <v>HQMbQQlWA5L</v>
       </c>
       <c r="E22" s="4" t="str">
-        <v>2019-05-10</v>
+        <v>2021-06-24</v>
       </c>
       <c r="F22" s="4" t="str">
-        <v>q9qKbXTDgEh</v>
+        <v>mN578Bop2g3</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="5" t="str">
-        <v>HIeML0i1tW6</v>
+        <v>W9BIjYTO9Py</v>
       </c>
       <c r="B23" s="5" t="str">
         <v>Chart</v>
       </c>
       <c r="C23" s="5" t="str">
-        <v>HIV - ART coverage - last month</v>
+        <v>HIV - HIV cascade by gender - last 12 months</v>
       </c>
       <c r="D23" s="5" t="str">
-        <v>FVRKyWnT7MK</v>
+        <v>cQPHqT5WT7k</v>
       </c>
       <c r="E23" s="5" t="str">
-        <v>2019-05-10</v>
+        <v>2021-06-24</v>
       </c>
       <c r="F23" s="5" t="str">
-        <v>q9qKbXTDgEh</v>
+        <v>mN578Bop2g3</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="4" t="str">
-        <v>yM52YmNwPdT</v>
+        <v>YRItoGE02Gc</v>
       </c>
       <c r="B24" s="4" t="str">
-        <v>Pivot table</v>
+        <v>Chart</v>
       </c>
       <c r="C24" s="4" t="str">
-        <v>HIV - HIV testing performance by sub-orgunits</v>
+        <v>HIV - 2nd and 3rd 90s</v>
       </c>
       <c r="D24" s="4" t="str">
-        <v>Jlt2k4A7zOK</v>
+        <v>Hn8SpMOfbkR</v>
       </c>
       <c r="E24" s="4" t="str">
-        <v>2019-05-10</v>
+        <v>2021-06-24</v>
       </c>
       <c r="F24" s="4" t="str">
-        <v>q9qKbXTDgEh</v>
+        <v>mN578Bop2g3</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="5" t="str">
-        <v>CInLEIQcstz</v>
+        <v>W5YurJlBYxS</v>
       </c>
       <c r="B25" s="5" t="str">
-        <v>Pivot table</v>
+        <v>Chart</v>
       </c>
       <c r="C25" s="5" t="str">
-        <v>HIV - ART performance by sub-orgunits</v>
+        <v>HIV - Trend in HIV testing</v>
       </c>
       <c r="D25" s="5" t="str">
-        <v>QfXeDVl4ONy</v>
+        <v>R9mBl80z4gR</v>
       </c>
       <c r="E25" s="5" t="str">
-        <v>2019-05-10</v>
+        <v>2021-06-24</v>
       </c>
       <c r="F25" s="5" t="str">
-        <v>q9qKbXTDgEh</v>
+        <v>mN578Bop2g3</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="4" t="str">
-        <v>FXLnt2rX2GF</v>
+        <v>neY7yCy63LJ</v>
       </c>
       <c r="B26" s="4" t="str">
-        <v>Pivot table</v>
+        <v>Chart</v>
       </c>
       <c r="C26" s="4" t="str">
-        <v>HIV - ART coverage by sub-orgunits</v>
+        <v>HIV - Trend in HIV test positivity</v>
       </c>
       <c r="D26" s="4" t="str">
-        <v>ribZrhKrUDJ</v>
+        <v>DhGugWmf82U</v>
       </c>
       <c r="E26" s="4" t="str">
-        <v>2019-05-10</v>
+        <v>2021-06-24</v>
       </c>
       <c r="F26" s="4" t="str">
-        <v>q9qKbXTDgEh</v>
+        <v>mN578Bop2g3</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="5" t="str">
-        <v>VFaZffBlMro</v>
+        <v>MlwuLdHcS0Y</v>
       </c>
       <c r="B27" s="5" t="str">
-        <v>Map</v>
+        <v>Chart</v>
       </c>
       <c r="C27" s="5" t="str">
-        <v>HIV - ART coverage</v>
+        <v>HIV - Trend in newly diagnosed and new on ART</v>
       </c>
       <c r="D27" s="5" t="str">
-        <v>RkiBAK4tecO</v>
+        <v>aOd1P9Jy9Bx</v>
       </c>
       <c r="E27" s="5" t="str">
-        <v>2019-05-10</v>
+        <v>2021-06-24</v>
       </c>
       <c r="F27" s="5" t="str">
-        <v>q9qKbXTDgEh</v>
+        <v>mN578Bop2g3</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="4" t="str">
-        <v>YLGtwHbfxqG</v>
+        <v>yZx4xQJ1AIt</v>
       </c>
       <c r="B28" s="4" t="str">
-        <v>Map</v>
+        <v>Chart</v>
       </c>
       <c r="C28" s="4" t="str">
-        <v>HIV - ART retention rate (12 months)</v>
+        <v>HIV - Trend in ART retention and VL suppression</v>
       </c>
       <c r="D28" s="4" t="str">
-        <v>YCl3k5LY0vQ</v>
+        <v>qCqeB2Is75g</v>
       </c>
       <c r="E28" s="4" t="str">
-        <v>2019-05-10</v>
+        <v>2021-06-24</v>
       </c>
       <c r="F28" s="4" t="str">
-        <v>q9qKbXTDgEh</v>
+        <v>mN578Bop2g3</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="5" t="str">
-        <v>MlwuLdHcS0Y</v>
+        <v>sbsctgkgtxi</v>
       </c>
       <c r="B29" s="5" t="str">
         <v>Chart</v>
       </c>
       <c r="C29" s="5" t="str">
-        <v>HIV - Trend in newly diagnosed and new on ART</v>
+        <v>HIV - HIV cascade</v>
       </c>
       <c r="D29" s="5" t="str">
-        <v>Dl6kcsXm54p</v>
+        <v>jnd7OXSZ3td</v>
       </c>
       <c r="E29" s="5" t="str">
         <v>2019-05-10</v>
@@ -2570,22 +3737,262 @@
     </row>
     <row r="30">
       <c r="A30" s="4" t="str">
-        <v>yZx4xQJ1AIt</v>
+        <v>W9BIjYTO9Py</v>
       </c>
       <c r="B30" s="4" t="str">
         <v>Chart</v>
       </c>
       <c r="C30" s="4" t="str">
-        <v>HIV - Trend in ART retention and VL suppression</v>
+        <v>HIV - HIV cascade by gender - last 12 months</v>
       </c>
       <c r="D30" s="4" t="str">
-        <v>ELciLRjAxS6</v>
+        <v>XnNRP887MgT</v>
       </c>
       <c r="E30" s="4" t="str">
         <v>2019-05-10</v>
       </c>
       <c r="F30" s="4" t="str">
         <v>q9qKbXTDgEh</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="5" t="str">
+        <v>YRItoGE02Gc</v>
+      </c>
+      <c r="B31" s="5" t="str">
+        <v>Chart</v>
+      </c>
+      <c r="C31" s="5" t="str">
+        <v>HIV - 2nd and 3rd 90s</v>
+      </c>
+      <c r="D31" s="5" t="str">
+        <v>Yybjz35BBy4</v>
+      </c>
+      <c r="E31" s="5" t="str">
+        <v>2019-05-10</v>
+      </c>
+      <c r="F31" s="5" t="str">
+        <v>q9qKbXTDgEh</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="4" t="str">
+        <v>HIeML0i1tW6</v>
+      </c>
+      <c r="B32" s="4" t="str">
+        <v>Chart</v>
+      </c>
+      <c r="C32" s="4" t="str">
+        <v>HIV - ART coverage - last month</v>
+      </c>
+      <c r="D32" s="4" t="str">
+        <v>FVRKyWnT7MK</v>
+      </c>
+      <c r="E32" s="4" t="str">
+        <v>2019-05-10</v>
+      </c>
+      <c r="F32" s="4" t="str">
+        <v>q9qKbXTDgEh</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="5" t="str">
+        <v>yM52YmNwPdT</v>
+      </c>
+      <c r="B33" s="5" t="str">
+        <v>Pivot table</v>
+      </c>
+      <c r="C33" s="5" t="str">
+        <v>HIV - HIV testing performance by sub-orgunits</v>
+      </c>
+      <c r="D33" s="5" t="str">
+        <v>Jlt2k4A7zOK</v>
+      </c>
+      <c r="E33" s="5" t="str">
+        <v>2019-05-10</v>
+      </c>
+      <c r="F33" s="5" t="str">
+        <v>q9qKbXTDgEh</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="4" t="str">
+        <v>CInLEIQcstz</v>
+      </c>
+      <c r="B34" s="4" t="str">
+        <v>Pivot table</v>
+      </c>
+      <c r="C34" s="4" t="str">
+        <v>HIV - ART performance by sub-orgunits</v>
+      </c>
+      <c r="D34" s="4" t="str">
+        <v>QfXeDVl4ONy</v>
+      </c>
+      <c r="E34" s="4" t="str">
+        <v>2019-05-10</v>
+      </c>
+      <c r="F34" s="4" t="str">
+        <v>q9qKbXTDgEh</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="5" t="str">
+        <v>FXLnt2rX2GF</v>
+      </c>
+      <c r="B35" s="5" t="str">
+        <v>Pivot table</v>
+      </c>
+      <c r="C35" s="5" t="str">
+        <v>HIV - ART coverage by sub-orgunits</v>
+      </c>
+      <c r="D35" s="5" t="str">
+        <v>ribZrhKrUDJ</v>
+      </c>
+      <c r="E35" s="5" t="str">
+        <v>2019-05-10</v>
+      </c>
+      <c r="F35" s="5" t="str">
+        <v>q9qKbXTDgEh</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="4" t="str">
+        <v>VFaZffBlMro</v>
+      </c>
+      <c r="B36" s="4" t="str">
+        <v>Map</v>
+      </c>
+      <c r="C36" s="4" t="str">
+        <v>HIV - ART coverage</v>
+      </c>
+      <c r="D36" s="4" t="str">
+        <v>RkiBAK4tecO</v>
+      </c>
+      <c r="E36" s="4" t="str">
+        <v>2019-05-10</v>
+      </c>
+      <c r="F36" s="4" t="str">
+        <v>q9qKbXTDgEh</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="5" t="str">
+        <v>YLGtwHbfxqG</v>
+      </c>
+      <c r="B37" s="5" t="str">
+        <v>Map</v>
+      </c>
+      <c r="C37" s="5" t="str">
+        <v>HIV - ART retention rate (12 months)</v>
+      </c>
+      <c r="D37" s="5" t="str">
+        <v>YCl3k5LY0vQ</v>
+      </c>
+      <c r="E37" s="5" t="str">
+        <v>2019-05-10</v>
+      </c>
+      <c r="F37" s="5" t="str">
+        <v>q9qKbXTDgEh</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="4" t="str">
+        <v>MlwuLdHcS0Y</v>
+      </c>
+      <c r="B38" s="4" t="str">
+        <v>Chart</v>
+      </c>
+      <c r="C38" s="4" t="str">
+        <v>HIV - Trend in newly diagnosed and new on ART</v>
+      </c>
+      <c r="D38" s="4" t="str">
+        <v>Dl6kcsXm54p</v>
+      </c>
+      <c r="E38" s="4" t="str">
+        <v>2019-05-10</v>
+      </c>
+      <c r="F38" s="4" t="str">
+        <v>q9qKbXTDgEh</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="5" t="str">
+        <v>yZx4xQJ1AIt</v>
+      </c>
+      <c r="B39" s="5" t="str">
+        <v>Chart</v>
+      </c>
+      <c r="C39" s="5" t="str">
+        <v>HIV - Trend in ART retention and VL suppression</v>
+      </c>
+      <c r="D39" s="5" t="str">
+        <v>ELciLRjAxS6</v>
+      </c>
+      <c r="E39" s="5" t="str">
+        <v>2019-05-10</v>
+      </c>
+      <c r="F39" s="5" t="str">
+        <v>q9qKbXTDgEh</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="4" t="str">
+        <v>Vf3ASwHkAmu</v>
+      </c>
+      <c r="B40" s="4" t="str">
+        <v>Map</v>
+      </c>
+      <c r="C40" s="4" t="str">
+        <v>GEN - Population estimate</v>
+      </c>
+      <c r="D40" s="4" t="str">
+        <v>bCMiCx5yJDZ</v>
+      </c>
+      <c r="E40" s="4" t="str">
+        <v>2019-05-10</v>
+      </c>
+      <c r="F40" s="4" t="str">
+        <v>VjFMk8X026U</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="5" t="str">
+        <v>t6lhTAiujEe</v>
+      </c>
+      <c r="B41" s="5" t="str">
+        <v>Map</v>
+      </c>
+      <c r="C41" s="5" t="str">
+        <v>HIV - PLHIV estimate</v>
+      </c>
+      <c r="D41" s="5" t="str">
+        <v>sXRmIoonkxp</v>
+      </c>
+      <c r="E41" s="5" t="str">
+        <v>2019-05-10</v>
+      </c>
+      <c r="F41" s="5" t="str">
+        <v>VjFMk8X026U</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="4" t="str">
+        <v>eu3QTttWA2p</v>
+      </c>
+      <c r="B42" s="4" t="str">
+        <v>Map</v>
+      </c>
+      <c r="C42" s="4" t="str">
+        <v>HIV - Estimated HIV prevalence</v>
+      </c>
+      <c r="D42" s="4" t="str">
+        <v>dDuqItmcL36</v>
+      </c>
+      <c r="E42" s="4" t="str">
+        <v>2019-05-10</v>
+      </c>
+      <c r="F42" s="4" t="str">
+        <v>VjFMk8X026U</v>
       </c>
     </row>
   </sheetData>

</xml_diff>